<commit_message>
Small changes in text
</commit_message>
<xml_diff>
--- a/Results/ANN (DE, PSO, UMDA, DEDA).xlsx
+++ b/Results/ANN (DE, PSO, UMDA, DEDA).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="540" windowWidth="25340" windowHeight="16380"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="24320" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="FIT" sheetId="1" r:id="rId1"/>
@@ -120,11 +120,11 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -414,22 +414,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -459,231 +459,199 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>15.933841825867692</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.9860273225978185E-15</v>
+        <v>15.333453060715755</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>15.333453060715755</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>15.404104106162331</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3.5166028006858287E-2</v>
+        <v>15.524891059342343</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.10793285726290715</v>
       </c>
       <c r="G3" s="1">
-        <v>15.467560982154016</v>
-      </c>
-      <c r="H3" s="2">
-        <v>5.9998544930906686E-2</v>
+        <v>15.333453060716749</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2.2267341529379978E-12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>45.103580681488545</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.8599117675150136E-4</v>
+        <v>199.6030061177791</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.6100158977057181E-4</v>
       </c>
       <c r="C4" s="1">
-        <v>45.101747665788842</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
+        <v>199.60420634922809</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.8732851388176597E-4</v>
       </c>
       <c r="E4" s="1">
-        <v>45.101747665992875</v>
-      </c>
-      <c r="F4" s="2">
-        <v>4.2215586191323777E-10</v>
+        <v>199.6046031746032</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.8421709430404007E-14</v>
       </c>
       <c r="G4" s="1">
-        <v>45.101747668325388</v>
-      </c>
-      <c r="H4" s="2">
-        <v>4.2051366382361111E-9</v>
+        <v>199.60301587272761</v>
+      </c>
+      <c r="H4" s="1">
+        <v>8.8732790601123363E-4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>199.60464352400854</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4.7025063873261841E-5</v>
+        <v>127291.00401606425</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>199.60420634945839</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8.8732799891282532E-4</v>
+        <v>127291.00401606425</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>199.60460317460317</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
+        <v>127291.0040160887</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5.1357248764017916E-8</v>
       </c>
       <c r="G5" s="1">
-        <v>199.6046031746032</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2.8421709430404007E-14</v>
+        <v>127291.00401606425</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>6.4858373473614117E-3</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9.5641671445974839E-4</v>
+        <v>4535.8819444444443</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>8.1102318312732471E-3</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.3275963426550605E-3</v>
+        <v>4535.8819444444443</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>6.8534913105785826E-3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>3.6193750738813791E-4</v>
+        <v>4535.8838383252532</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7.0180116077090753E-8</v>
       </c>
       <c r="G6" s="1">
-        <v>6.6724676295941256E-3</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2.870127749949898E-4</v>
+        <v>4535.8819444444443</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>127291.06629365189</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1.7591607490120411E-5</v>
+        <v>502053.26589279092</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5.0857770806125913E-2</v>
       </c>
       <c r="C7" s="1">
-        <v>127291.00401606425</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
+        <v>502056.5035258549</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.8213603576168393</v>
       </c>
       <c r="E7" s="1">
-        <v>127291.00401606574</v>
-      </c>
-      <c r="F7" s="2">
-        <v>3.3010964368076531E-9</v>
+        <v>502058.49627535336</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.97348043596611722</v>
       </c>
       <c r="G7" s="1">
-        <v>127291.00401606466</v>
-      </c>
-      <c r="H7" s="2">
-        <v>6.4858132676647951E-10</v>
+        <v>502053.24884617608</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1.5735821426437174E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>4535.8849132198056</v>
-      </c>
-      <c r="B8" s="2">
-        <v>9.1258966741421515E-4</v>
+        <v>274.04065217391292</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>4535.8819444444443</v>
-      </c>
-      <c r="D8" s="2">
+        <v>274.04065217391292</v>
+      </c>
+      <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>4535.8838383838383</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0168459891700831E-12</v>
+        <v>274.04065217391292</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.8421709430404007E-14</v>
       </c>
       <c r="G8" s="1">
-        <v>4535.8838383814164</v>
-      </c>
-      <c r="H8" s="2">
-        <v>3.3203227648705981E-9</v>
+        <v>274.04065217391292</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>502097.5101952207</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.3824157905271417</v>
-      </c>
-      <c r="C9" s="1">
-        <v>502054.88653894188</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2.2196834037184088</v>
-      </c>
-      <c r="E9" s="1">
-        <v>502058.72408979264</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.90635155388283284</v>
-      </c>
-      <c r="G9" s="1">
-        <v>502058.27243218094</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.42535717934997319</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>274.04068554891808</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2.1509279496310604E-5</v>
-      </c>
-      <c r="C10" s="1">
-        <v>274.04065217391292</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>274.04065217391309</v>
-      </c>
-      <c r="F10" s="2">
-        <v>3.2530133302826691E-13</v>
-      </c>
-      <c r="G10" s="1">
-        <v>274.04065217391292</v>
-      </c>
-      <c r="H10" s="2">
-        <v>4.0194366942304644E-14</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>